<commit_message>
Subindo códigos testados suas descrições
</commit_message>
<xml_diff>
--- a/DadosAcoesTreinee.xlsx
+++ b/DadosAcoesTreinee.xlsx
@@ -492,7 +492,7 @@
         <v>119662</v>
       </c>
       <c r="H2" t="n">
-        <v>119630</v>
+        <v>121341.1328125</v>
       </c>
     </row>
     <row r="3">
@@ -548,7 +548,7 @@
         <v>20.95999908447266</v>
       </c>
       <c r="H4" t="n">
-        <v>20.79999923706055</v>
+        <v>20.93000030517578</v>
       </c>
     </row>
     <row r="5">
@@ -576,7 +576,7 @@
         <v>11.23999977111816</v>
       </c>
       <c r="H5" t="n">
-        <v>11.25</v>
+        <v>11.27999973297119</v>
       </c>
     </row>
     <row r="6">
@@ -604,7 +604,7 @@
         <v>46.5</v>
       </c>
       <c r="H6" t="n">
-        <v>46.34000015258789</v>
+        <v>47.40999984741211</v>
       </c>
     </row>
     <row r="7">
@@ -632,7 +632,7 @@
         <v>29.48999977111816</v>
       </c>
       <c r="H7" t="n">
-        <v>29.56999969482422</v>
+        <v>30.04000091552734</v>
       </c>
     </row>
     <row r="8">
@@ -660,7 +660,7 @@
         <v>50.2599983215332</v>
       </c>
       <c r="H8" t="n">
-        <v>50.18999862670898</v>
+        <v>49.59000015258789</v>
       </c>
     </row>
     <row r="9">
@@ -670,25 +670,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10.9399995803833</v>
+        <v>10.85123538970947</v>
       </c>
       <c r="C9" t="n">
-        <v>11.42000007629395</v>
+        <v>11.32734107971191</v>
       </c>
       <c r="D9" t="n">
-        <v>11.14000034332275</v>
+        <v>11.0496129989624</v>
       </c>
       <c r="E9" t="n">
-        <v>10.69999980926514</v>
+        <v>10.61318302154541</v>
       </c>
       <c r="F9" t="n">
-        <v>10.75</v>
+        <v>10.66277694702148</v>
       </c>
       <c r="G9" t="n">
-        <v>10.36999988555908</v>
+        <v>10.28586006164551</v>
       </c>
       <c r="H9" t="n">
-        <v>10.60999965667725</v>
+        <v>10.39000034332275</v>
       </c>
     </row>
     <row r="10">
@@ -716,7 +716,7 @@
         <v>89.40000152587891</v>
       </c>
       <c r="H10" t="n">
-        <v>88.65000152587891</v>
+        <v>88.98999786376953</v>
       </c>
     </row>
     <row r="11">
@@ -729,7 +729,7 @@
         <v>26.95261764526367</v>
       </c>
       <c r="C11" t="n">
-        <v>27.02092552185059</v>
+        <v>27.02092742919922</v>
       </c>
       <c r="D11" t="n">
         <v>26.4256649017334</v>
@@ -744,7 +744,7 @@
         <v>26.45000076293945</v>
       </c>
       <c r="H11" t="n">
-        <v>26.07999992370605</v>
+        <v>26.61000061035156</v>
       </c>
     </row>
     <row r="12">
@@ -754,25 +754,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12.94346904754639</v>
+        <v>13.35010242462158</v>
       </c>
       <c r="C12" t="n">
-        <v>13.00155544281006</v>
+        <v>13.41001319885254</v>
       </c>
       <c r="D12" t="n">
-        <v>12.55623054504395</v>
+        <v>12.95069789886475</v>
       </c>
       <c r="E12" t="n">
-        <v>12.26580047607422</v>
+        <v>12.65114402770996</v>
       </c>
       <c r="F12" t="n">
-        <v>12.5555534362793</v>
+        <v>12.94999980926514</v>
       </c>
       <c r="G12" t="n">
-        <v>12.439208984375</v>
+        <v>12.82999992370605</v>
       </c>
       <c r="H12" t="n">
-        <v>12.38000011444092</v>
+        <v>12.39999961853027</v>
       </c>
     </row>
     <row r="13">
@@ -800,7 +800,7 @@
         <v>24.84000015258789</v>
       </c>
       <c r="H13" t="n">
-        <v>25.59000015258789</v>
+        <v>24.93000030517578</v>
       </c>
     </row>
     <row r="14">
@@ -828,7 +828,7 @@
         <v>31.89999961853027</v>
       </c>
       <c r="H14" t="n">
-        <v>31.94000053405762</v>
+        <v>32.47999954223633</v>
       </c>
     </row>
     <row r="15">
@@ -856,7 +856,7 @@
         <v>18.6299991607666</v>
       </c>
       <c r="H15" t="n">
-        <v>19.19000053405762</v>
+        <v>20.54999923706055</v>
       </c>
     </row>
     <row r="16">
@@ -884,7 +884,7 @@
         <v>11.59000015258789</v>
       </c>
       <c r="H16" t="n">
-        <v>11.43000030517578</v>
+        <v>12.02999973297119</v>
       </c>
     </row>
     <row r="17">
@@ -912,7 +912,7 @@
         <v>1.669999957084656</v>
       </c>
       <c r="H17" t="n">
-        <v>1.639999985694885</v>
+        <v>1.740000009536743</v>
       </c>
     </row>
     <row r="18">
@@ -940,7 +940,7 @@
         <v>12.67000007629395</v>
       </c>
       <c r="H18" t="n">
-        <v>12.48999977111816</v>
+        <v>12.89000034332275</v>
       </c>
     </row>
     <row r="19">
@@ -968,7 +968,7 @@
         <v>2.009999990463257</v>
       </c>
       <c r="H19" t="n">
-        <v>1.909999966621399</v>
+        <v>1.899999976158142</v>
       </c>
     </row>
     <row r="20">
@@ -996,7 +996,7 @@
         <v>15.3100004196167</v>
       </c>
       <c r="H20" t="n">
-        <v>14.57999992370605</v>
+        <v>14.78999996185303</v>
       </c>
     </row>
     <row r="21">
@@ -1024,7 +1024,7 @@
         <v>37.33000183105469</v>
       </c>
       <c r="H21" t="n">
-        <v>36.79999923706055</v>
+        <v>37.86999893188477</v>
       </c>
     </row>
     <row r="22">
@@ -1052,7 +1052,7 @@
         <v>13.30000019073486</v>
       </c>
       <c r="H22" t="n">
-        <v>12.85999965667725</v>
+        <v>12.89999961853027</v>
       </c>
     </row>
     <row r="23">
@@ -1080,7 +1080,7 @@
         <v>14.19999980926514</v>
       </c>
       <c r="H23" t="n">
-        <v>14.02000045776367</v>
+        <v>14.21000003814697</v>
       </c>
     </row>
     <row r="24">
@@ -1108,7 +1108,7 @@
         <v>17</v>
       </c>
       <c r="H24" t="n">
-        <v>16.97999954223633</v>
+        <v>17.73999977111816</v>
       </c>
     </row>
     <row r="25">
@@ -1136,7 +1136,7 @@
         <v>7.198954105377197</v>
       </c>
       <c r="H25" t="n">
-        <v>7.159999847412109</v>
+        <v>7.150000095367432</v>
       </c>
     </row>
     <row r="26">
@@ -1164,7 +1164,7 @@
         <v>3.619999885559082</v>
       </c>
       <c r="H26" t="n">
-        <v>3.440000057220459</v>
+        <v>3.769999980926514</v>
       </c>
     </row>
     <row r="27">
@@ -1192,7 +1192,7 @@
         <v>109.9800033569336</v>
       </c>
       <c r="H27" t="n">
-        <v>110.0899963378906</v>
+        <v>110.0800018310547</v>
       </c>
     </row>
     <row r="28">
@@ -1220,7 +1220,7 @@
         <v>19.55999946594238</v>
       </c>
       <c r="H28" t="n">
-        <v>19.36000061035156</v>
+        <v>19.71999931335449</v>
       </c>
     </row>
     <row r="29">
@@ -1248,7 +1248,7 @@
         <v>97.83000183105469</v>
       </c>
       <c r="H29" t="n">
-        <v>98.02999877929688</v>
+        <v>98.36000061035156</v>
       </c>
     </row>
     <row r="30">
@@ -1276,7 +1276,7 @@
         <v>82.51000213623047</v>
       </c>
       <c r="H30" t="n">
-        <v>82.40000152587891</v>
+        <v>82.62000274658203</v>
       </c>
     </row>
     <row r="31">
@@ -1286,25 +1286,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>10.01572036743164</v>
+        <v>9.919038772583008</v>
       </c>
       <c r="C31" t="n">
-        <v>10.23518848419189</v>
+        <v>10.13638782501221</v>
       </c>
       <c r="D31" t="n">
-        <v>9.935914039611816</v>
+        <v>9.84000301361084</v>
       </c>
       <c r="E31" t="n">
-        <v>9.706469535827637</v>
+        <v>9.612772941589355</v>
       </c>
       <c r="F31" t="n">
-        <v>9.699999809265137</v>
+        <v>9.606365203857422</v>
       </c>
       <c r="G31" t="n">
-        <v>9.569999694824219</v>
+        <v>9.477620124816895</v>
       </c>
       <c r="H31" t="n">
-        <v>9.710000038146973</v>
+        <v>9.680000305175781</v>
       </c>
     </row>
     <row r="32">
@@ -1314,22 +1314,22 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>32.63143157958984</v>
+        <v>32.374755859375</v>
       </c>
       <c r="C32" t="n">
-        <v>33.21109771728516</v>
+        <v>32.94986343383789</v>
       </c>
       <c r="D32" t="n">
-        <v>31.83188438415527</v>
+        <v>31.58149909973145</v>
       </c>
       <c r="E32" t="n">
-        <v>31.01235008239746</v>
+        <v>30.76841163635254</v>
       </c>
       <c r="F32" t="n">
-        <v>31.45000076293945</v>
+        <v>31.2026195526123</v>
       </c>
       <c r="G32" t="n">
-        <v>31.13999938964844</v>
+        <v>30.89505767822266</v>
       </c>
       <c r="H32" t="n">
         <v>31.8799991607666</v>
@@ -1360,7 +1360,7 @@
         <v>28.61000061035156</v>
       </c>
       <c r="H33" t="n">
-        <v>28.89999961853027</v>
+        <v>30.67000007629395</v>
       </c>
     </row>
     <row r="34">
@@ -1388,7 +1388,7 @@
         <v>4.070000171661377</v>
       </c>
       <c r="H34" t="n">
-        <v>4.110000133514404</v>
+        <v>4.190000057220459</v>
       </c>
     </row>
     <row r="35">
@@ -1416,7 +1416,7 @@
         <v>12.78999996185303</v>
       </c>
       <c r="H35" t="n">
-        <v>12.35999965667725</v>
+        <v>12.52999973297119</v>
       </c>
     </row>
     <row r="36">
@@ -1444,7 +1444,7 @@
         <v>4.199999809265137</v>
       </c>
       <c r="H36" t="n">
-        <v>3.980000019073486</v>
+        <v>3.990000009536743</v>
       </c>
     </row>
     <row r="37">
@@ -1472,7 +1472,7 @@
         <v>70.36000061035156</v>
       </c>
       <c r="H37" t="n">
-        <v>70.91999816894531</v>
+        <v>72.23999786376953</v>
       </c>
     </row>
     <row r="38">
@@ -1500,7 +1500,7 @@
         <v>6.03000020980835</v>
       </c>
       <c r="H38" t="n">
-        <v>5.809999942779541</v>
+        <v>5.940000057220459</v>
       </c>
     </row>
     <row r="39">
@@ -1528,7 +1528,7 @@
         <v>10.52000045776367</v>
       </c>
       <c r="H39" t="n">
-        <v>10.5600004196167</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="40">
@@ -1556,7 +1556,7 @@
         <v>5.440000057220459</v>
       </c>
       <c r="H40" t="n">
-        <v>5.269999980926514</v>
+        <v>5.210000038146973</v>
       </c>
     </row>
     <row r="41">
@@ -1584,7 +1584,7 @@
         <v>34.68000030517578</v>
       </c>
       <c r="H41" t="n">
-        <v>35.90000152587891</v>
+        <v>36.72000122070312</v>
       </c>
     </row>
     <row r="42">
@@ -1612,7 +1612,7 @@
         <v>3.5</v>
       </c>
       <c r="H42" t="n">
-        <v>3.319999933242798</v>
+        <v>3.450000047683716</v>
       </c>
     </row>
     <row r="43">
@@ -1640,7 +1640,7 @@
         <v>14.55000019073486</v>
       </c>
       <c r="H43" t="n">
-        <v>14.47000026702881</v>
+        <v>14.63000011444092</v>
       </c>
     </row>
     <row r="44">
@@ -1668,7 +1668,7 @@
         <v>42.0099983215332</v>
       </c>
       <c r="H44" t="n">
-        <v>41.25</v>
+        <v>41.33000183105469</v>
       </c>
     </row>
     <row r="45">
@@ -1696,7 +1696,7 @@
         <v>19.77000045776367</v>
       </c>
       <c r="H45" t="n">
-        <v>19.5</v>
+        <v>20.04999923706055</v>
       </c>
     </row>
     <row r="46">
@@ -1724,7 +1724,7 @@
         <v>26.93000030517578</v>
       </c>
       <c r="H46" t="n">
-        <v>26.20000076293945</v>
+        <v>26.35000038146973</v>
       </c>
     </row>
     <row r="47">
@@ -1752,7 +1752,7 @@
         <v>10.43000030517578</v>
       </c>
       <c r="H47" t="n">
-        <v>10.5600004196167</v>
+        <v>11.09000015258789</v>
       </c>
     </row>
     <row r="48">
@@ -1780,7 +1780,7 @@
         <v>25.89999961853027</v>
       </c>
       <c r="H48" t="n">
-        <v>25.39999961853027</v>
+        <v>25.61000061035156</v>
       </c>
     </row>
     <row r="49">
@@ -1808,7 +1808,7 @@
         <v>17.6299991607666</v>
       </c>
       <c r="H49" t="n">
-        <v>17.52000045776367</v>
+        <v>17.45999908447266</v>
       </c>
     </row>
     <row r="50">
@@ -1818,25 +1818,25 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>28.29000091552734</v>
+        <v>27.90649223327637</v>
       </c>
       <c r="C50" t="n">
-        <v>27.03000068664551</v>
+        <v>26.66357231140137</v>
       </c>
       <c r="D50" t="n">
-        <v>26.90999984741211</v>
+        <v>26.54519844055176</v>
       </c>
       <c r="E50" t="n">
-        <v>27.13999938964844</v>
+        <v>26.77207946777344</v>
       </c>
       <c r="F50" t="n">
-        <v>28.25</v>
+        <v>27.86703300476074</v>
       </c>
       <c r="G50" t="n">
-        <v>30.73999977111816</v>
+        <v>30.32327651977539</v>
       </c>
       <c r="H50" t="n">
-        <v>30.86000061035156</v>
+        <v>32.36999893188477</v>
       </c>
     </row>
     <row r="51">
@@ -1864,7 +1864,7 @@
         <v>5.900000095367432</v>
       </c>
       <c r="H51" t="n">
-        <v>5.820000171661377</v>
+        <v>5.860000133514404</v>
       </c>
     </row>
     <row r="52">
@@ -1892,7 +1892,7 @@
         <v>48.97000122070312</v>
       </c>
       <c r="H52" t="n">
-        <v>48.29999923706055</v>
+        <v>48.84999847412109</v>
       </c>
     </row>
     <row r="53">
@@ -1920,7 +1920,7 @@
         <v>33.34999847412109</v>
       </c>
       <c r="H53" t="n">
-        <v>33.29000091552734</v>
+        <v>33.59999847412109</v>
       </c>
     </row>
     <row r="54">
@@ -1948,7 +1948,7 @@
         <v>15.86999988555908</v>
       </c>
       <c r="H54" t="n">
-        <v>15.6899995803833</v>
+        <v>15.77999973297119</v>
       </c>
     </row>
     <row r="55">
@@ -1976,7 +1976,7 @@
         <v>60.61999893188477</v>
       </c>
       <c r="H55" t="n">
-        <v>60.65999984741211</v>
+        <v>60.83000183105469</v>
       </c>
     </row>
     <row r="56">
@@ -2004,7 +2004,7 @@
         <v>5.449999809265137</v>
       </c>
       <c r="H56" t="n">
-        <v>5.449999809265137</v>
+        <v>5.820000171661377</v>
       </c>
     </row>
     <row r="57">
@@ -2032,7 +2032,7 @@
         <v>44.90000152587891</v>
       </c>
       <c r="H57" t="n">
-        <v>44.33000183105469</v>
+        <v>44.4900016784668</v>
       </c>
     </row>
     <row r="58">
@@ -2060,7 +2060,7 @@
         <v>38.77000045776367</v>
       </c>
       <c r="H58" t="n">
-        <v>38.86000061035156</v>
+        <v>41.08000183105469</v>
       </c>
     </row>
     <row r="59">
@@ -2088,7 +2088,7 @@
         <v>11.22000026702881</v>
       </c>
       <c r="H59" t="n">
-        <v>10.63000011444092</v>
+        <v>10.84000015258789</v>
       </c>
     </row>
     <row r="60">
@@ -2116,7 +2116,7 @@
         <v>542.780029296875</v>
       </c>
       <c r="H60" t="n">
-        <v>548.489990234375</v>
+        <v>544.510009765625</v>
       </c>
     </row>
     <row r="61">
@@ -2144,7 +2144,7 @@
         <v>88.98000335693359</v>
       </c>
       <c r="H61" t="n">
-        <v>89.54000091552734</v>
+        <v>89.63999938964844</v>
       </c>
     </row>
     <row r="62">
@@ -2172,7 +2172,7 @@
         <v>40.65000152587891</v>
       </c>
       <c r="H62" t="n">
-        <v>41.27000045776367</v>
+        <v>41.33000183105469</v>
       </c>
     </row>
     <row r="63">
@@ -2200,7 +2200,7 @@
         <v>121.1500015258789</v>
       </c>
       <c r="H63" t="n">
-        <v>123.1500015258789</v>
+        <v>122.9700012207031</v>
       </c>
     </row>
     <row r="64">
@@ -2228,7 +2228,7 @@
         <v>227.6699981689453</v>
       </c>
       <c r="H64" t="n">
-        <v>231.4100036621094</v>
+        <v>228.4100036621094</v>
       </c>
     </row>
     <row r="65">
@@ -2256,7 +2256,7 @@
         <v>76.94999694824219</v>
       </c>
       <c r="H65" t="n">
-        <v>77.77999877929688</v>
+        <v>77.66999816894531</v>
       </c>
     </row>
     <row r="66">
@@ -2284,7 +2284,7 @@
         <v>69.94000244140625</v>
       </c>
       <c r="H66" t="n">
-        <v>69.19999694824219</v>
+        <v>69.38999938964844</v>
       </c>
     </row>
     <row r="67">
@@ -2312,7 +2312,7 @@
         <v>145.8800048828125</v>
       </c>
       <c r="H67" t="n">
-        <v>145.9199981689453</v>
+        <v>146.8099975585938</v>
       </c>
     </row>
     <row r="68">
@@ -2340,7 +2340,7 @@
         <v>178.3300018310547</v>
       </c>
       <c r="H68" t="n">
-        <v>180.8500061035156</v>
+        <v>182.6100006103516</v>
       </c>
     </row>
     <row r="69">
@@ -2368,7 +2368,7 @@
         <v>75.05999755859375</v>
       </c>
       <c r="H69" t="n">
-        <v>75.86000061035156</v>
+        <v>77.04360198974609</v>
       </c>
     </row>
     <row r="70">
@@ -2396,7 +2396,7 @@
         <v>67.12999725341797</v>
       </c>
       <c r="H70" t="n">
-        <v>66.66000366210938</v>
+        <v>66.01000213623047</v>
       </c>
     </row>
     <row r="71">
@@ -2424,7 +2424,7 @@
         <v>30.01000022888184</v>
       </c>
       <c r="H71" t="n">
-        <v>30.29000091552734</v>
+        <v>30.18000030517578</v>
       </c>
     </row>
     <row r="72">
@@ -2452,7 +2452,7 @@
         <v>42.22999954223633</v>
       </c>
       <c r="H72" t="n">
-        <v>42.88999938964844</v>
+        <v>42.66999816894531</v>
       </c>
     </row>
     <row r="73">
@@ -2480,7 +2480,7 @@
         <v>94.66999816894531</v>
       </c>
       <c r="H73" t="n">
-        <v>94.58999633789062</v>
+        <v>93.95999908447266</v>
       </c>
     </row>
     <row r="74">
@@ -2508,7 +2508,7 @@
         <v>215.7299957275391</v>
       </c>
       <c r="H74" t="n">
-        <v>215.4700012207031</v>
+        <v>214.7799987792969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>